<commit_message>
schematics Pr1, PBD 1
</commit_message>
<xml_diff>
--- a/Schematics/Book1.xlsx
+++ b/Schematics/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4th_semestr\fourth_semestr\Schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBAF25A-B06B-48B3-9EAE-91EFC4323FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B46C3B-1DF4-43C8-8475-9087AFB7D1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{DA204F5A-8798-413B-8F26-AFC921F08140}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{DA204F5A-8798-413B-8F26-AFC921F08140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="21">
   <si>
     <t>Состояние/входы</t>
   </si>
@@ -461,7 +461,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +504,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -534,9 +534,6 @@
       </c>
       <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -743,10 +740,13 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>